<commit_message>
Thêm testcase chỉnh sửa thông tin
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -171,6 +171,82 @@
   </si>
   <si>
     <t>Đăng ký</t>
+  </si>
+  <si>
+    <t>Chỉnh Sửa Thông Tin Cá Nhân Tài Khoản</t>
+  </si>
+  <si>
+    <t>009 - 001</t>
+  </si>
+  <si>
+    <t>Không thay đổi thông tin</t>
+  </si>
+  <si>
+    <t>Nhấn nút Update</t>
+  </si>
+  <si>
+    <t>1. Thông báo không có gì thay đổi và
+2. Không thực hiện tác vụ nào</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>009 -002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không nhập địa chỉ </t>
+  </si>
+  <si>
+    <t>1. Sửa tên:""
+2.Sửa địa chỉ:""
+3.Sửa số điện thoại:"+84915897496"</t>
+  </si>
+  <si>
+    <t>1. Không cho người dùng chỉnh sửa
+2. Thông báo lỗi tương ứng</t>
+  </si>
+  <si>
+    <t>009 - 003</t>
+  </si>
+  <si>
+    <t>Không nhập số điện thoại</t>
+  </si>
+  <si>
+    <t>1. Sửa tên:""
+2.Sửa địa chỉ:"227 Ho Tung Mau Q.PN"
+3.Sửa số điện thoại:""</t>
+  </si>
+  <si>
+    <t>009 - 004</t>
+  </si>
+  <si>
+    <t>Nhập số điện thoại không hợp lệ</t>
+  </si>
+  <si>
+    <t>1. Sửa tên:""
+2.Sửa địa chỉ:"227 Ho Tung Mau Q.PN"
+3.Sửa số điện thoại:"abc"</t>
+  </si>
+  <si>
+    <t>009 - 005</t>
+  </si>
+  <si>
+    <t>Chỉnh sửa hợp lệ</t>
+  </si>
+  <si>
+    <t>1. Sửa tên:""
+2.Sửa địa chỉ:"227 Ho Tung Mau Q.PN"
+3.Sửa số điện thoại:"+84915897496"</t>
+  </si>
+  <si>
+    <t>Cập nhật thông tin tài khoản và chuyển sang màn hình khác</t>
+  </si>
+  <si>
+    <t>Function 03</t>
+  </si>
+  <si>
+    <t>Thiện</t>
   </si>
 </sst>
 </file>
@@ -333,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -433,6 +509,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,13 +819,13 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="26" width="7.7109375" customWidth="1"/>
@@ -778,8 +866,12 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
@@ -6768,14 +6860,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" customWidth="1"/>
@@ -7374,16 +7466,20 @@
       <c r="Z17" s="8"/>
     </row>
     <row r="18" spans="1:26">
-      <c r="A18" s="28"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
+      <c r="A18" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
@@ -7402,15 +7498,32 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="60" customHeight="1">
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="28"/>
+      <c r="A19" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="44">
+        <v>42650</v>
+      </c>
+      <c r="J19" s="42"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -7429,16 +7542,32 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="60" customHeight="1">
-      <c r="A20" s="28"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="30"/>
-      <c r="J20" s="28"/>
+      <c r="A20" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="42"/>
+      <c r="D20" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" s="44">
+        <v>42650</v>
+      </c>
+      <c r="J20" s="42"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
@@ -7457,16 +7586,32 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="60" customHeight="1">
-      <c r="A21" s="28"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="28"/>
+      <c r="A21" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="44">
+        <v>42650</v>
+      </c>
+      <c r="J21" s="42"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -7485,16 +7630,32 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="60" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="28"/>
+      <c r="A22" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H22" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" s="44">
+        <v>42650</v>
+      </c>
+      <c r="J22" s="42"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -7512,17 +7673,33 @@
       <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
     </row>
-    <row r="23" spans="1:26">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
+    <row r="23" spans="1:26" ht="75">
+      <c r="A23" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="I23" s="44">
+        <v>42650</v>
+      </c>
+      <c r="J23" s="42"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>

</xml_diff>

<commit_message>
Thêm file xem cart, thêm test case logout
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>Remark</t>
-  </si>
-  <si>
-    <t>Đăng Nhập</t>
   </si>
   <si>
     <t>Test case name</t>
@@ -167,16 +164,10 @@
     <t>Chuyển sang phần đăng ký 2</t>
   </si>
   <si>
-    <t>Đăng Ký</t>
-  </si>
-  <si>
     <t>Đăng ký</t>
   </si>
   <si>
     <t>Chỉnh Sửa Thông Tin Cá Nhân Tài Khoản</t>
-  </si>
-  <si>
-    <t>009 - 001</t>
   </si>
   <si>
     <t>Không thay đổi thông tin</t>
@@ -192,9 +183,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>009 -002</t>
-  </si>
-  <si>
     <t xml:space="preserve">Không nhập địa chỉ </t>
   </si>
   <si>
@@ -207,9 +195,6 @@
 2. Thông báo lỗi tương ứng</t>
   </si>
   <si>
-    <t>009 - 003</t>
-  </si>
-  <si>
     <t>Không nhập số điện thoại</t>
   </si>
   <si>
@@ -218,18 +203,12 @@
 3.Sửa số điện thoại:""</t>
   </si>
   <si>
-    <t>009 - 004</t>
-  </si>
-  <si>
     <t>Nhập số điện thoại không hợp lệ</t>
   </si>
   <si>
     <t>1. Sửa tên:""
 2.Sửa địa chỉ:"227 Ho Tung Mau Q.PN"
 3.Sửa số điện thoại:"abc"</t>
-  </si>
-  <si>
-    <t>009 - 005</t>
   </si>
   <si>
     <t>Chỉnh sửa hợp lệ</t>
@@ -247,6 +226,30 @@
   </si>
   <si>
     <t>Thiện</t>
+  </si>
+  <si>
+    <t>Đăng xuất</t>
+  </si>
+  <si>
+    <t>Function 04</t>
+  </si>
+  <si>
+    <t>003 - 001</t>
+  </si>
+  <si>
+    <t>004 - 001</t>
+  </si>
+  <si>
+    <t>Nhấn nút Log out</t>
+  </si>
+  <si>
+    <t>1. Đăng xuất người dùng</t>
+  </si>
+  <si>
+    <t>Đăng xuất người dùng</t>
+  </si>
+  <si>
+    <t>15/7/2016</t>
   </si>
 </sst>
 </file>
@@ -409,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -521,6 +524,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -819,7 +829,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -849,8 +859,8 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
+      <c r="B2" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -860,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -869,15 +879,19 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>51</v>
+      <c r="B4" s="46" t="s">
+        <v>49</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>66</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
@@ -6860,8 +6874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -6882,28 +6896,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>3</v>
@@ -6927,10 +6941,10 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -6959,15 +6973,15 @@
     </row>
     <row r="3" spans="1:26" ht="45" customHeight="1">
       <c r="A3" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13"/>
@@ -6993,15 +7007,15 @@
     </row>
     <row r="4" spans="1:26" ht="55.5" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="13"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -7027,15 +7041,15 @@
     </row>
     <row r="5" spans="1:26" ht="56.25" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
@@ -7061,15 +7075,15 @@
     </row>
     <row r="6" spans="1:26" ht="67.5" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -7095,15 +7109,15 @@
     </row>
     <row r="7" spans="1:26" ht="57" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -7129,15 +7143,15 @@
     </row>
     <row r="8" spans="1:26" ht="57" customHeight="1">
       <c r="A8" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
@@ -7163,10 +7177,10 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
@@ -7195,15 +7209,15 @@
     </row>
     <row r="10" spans="1:26" ht="65.25" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13"/>
@@ -7229,15 +7243,15 @@
     </row>
     <row r="11" spans="1:26" ht="68.25" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -7263,15 +7277,15 @@
     </row>
     <row r="12" spans="1:26" ht="57.75" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -7297,15 +7311,15 @@
     </row>
     <row r="13" spans="1:26" ht="56.25" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="11"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -7331,15 +7345,15 @@
     </row>
     <row r="14" spans="1:26" ht="56.25" customHeight="1">
       <c r="A14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -7365,15 +7379,15 @@
     </row>
     <row r="15" spans="1:26" ht="67.5" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -7399,15 +7413,15 @@
     </row>
     <row r="16" spans="1:26" ht="81.75" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -7433,15 +7447,15 @@
     </row>
     <row r="17" spans="1:26" ht="68.25" customHeight="1">
       <c r="A17" s="39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="39"/>
       <c r="D17" s="40"/>
       <c r="E17" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="40"/>
       <c r="G17" s="40"/>
@@ -7467,10 +7481,10 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="26" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -7498,27 +7512,27 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="60" customHeight="1">
-      <c r="A19" s="42" t="s">
-        <v>52</v>
+      <c r="A19" s="47" t="s">
+        <v>68</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C19" s="42"/>
       <c r="D19" s="43" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F19" s="43" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I19" s="44">
         <v>42650</v>
@@ -7542,27 +7556,27 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" spans="1:26" ht="60" customHeight="1">
-      <c r="A20" s="42" t="s">
-        <v>57</v>
+      <c r="A20" s="47" t="s">
+        <v>68</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="43" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F20" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H20" s="45" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I20" s="44">
         <v>42650</v>
@@ -7586,27 +7600,27 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="60" customHeight="1">
-      <c r="A21" s="42" t="s">
-        <v>61</v>
+      <c r="A21" s="47" t="s">
+        <v>68</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="43" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G21" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I21" s="44">
         <v>42650</v>
@@ -7630,27 +7644,27 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="60" customHeight="1">
-      <c r="A22" s="42" t="s">
-        <v>64</v>
+      <c r="A22" s="47" t="s">
+        <v>68</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="43" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G22" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I22" s="44">
         <v>42650</v>
@@ -7674,27 +7688,27 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="75">
-      <c r="A23" s="42" t="s">
-        <v>67</v>
+      <c r="A23" s="47" t="s">
+        <v>68</v>
       </c>
       <c r="B23" s="42" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="43" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G23" s="43" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H23" s="45" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="I23" s="44">
         <v>42650</v>
@@ -7718,16 +7732,20 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" ht="54.75" customHeight="1">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="28"/>
+      <c r="A24" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
@@ -7746,16 +7764,32 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="60" customHeight="1">
-      <c r="A25" s="28"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="28"/>
+      <c r="A25" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="I25" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" s="42"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>

</xml_diff>

<commit_message>
Thêm testcase xem giỏ hàng
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -425,6 +425,54 @@
   <si>
     <t>006 - 004</t>
   </si>
+  <si>
+    <t>Xem giỏ hàng</t>
+  </si>
+  <si>
+    <t>Function 07</t>
+  </si>
+  <si>
+    <t>007-001</t>
+  </si>
+  <si>
+    <t>007-002</t>
+  </si>
+  <si>
+    <t>Xem giỏ hàng khi chưa đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Không đăng nhập
+2. Bấm vào nút xem giỏ hàng</t>
+  </si>
+  <si>
+    <t>1. Thông báo người phải đăng nhập để xem giỏ hàng</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập
+2. Bấm vào nút xem giỏ hàng</t>
+  </si>
+  <si>
+    <t>Xem giỏ hàng khi đã đăng nhập, chưa có hàng trong giỏ</t>
+  </si>
+  <si>
+    <t>1. Hiện giao diện giỏ hàng
+2. Thông báo rằng chưa có hàng trong giỏ</t>
+  </si>
+  <si>
+    <t>007-003</t>
+  </si>
+  <si>
+    <t>Xem giỏ hàng khi đã đăng nhập, đã có hàng trong giỏ</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập
+3. Thêm hàng vào giỏ
+2. Bấm vào nút xem giỏ hàng</t>
+  </si>
+  <si>
+    <t>1. Hiện giao diện giỏ hàng
+2. Hiển thị thông tin của hàng trong giỏ, số lượng và tổng giá tiền</t>
+  </si>
 </sst>
 </file>
 
@@ -615,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -689,9 +737,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -743,6 +788,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,7 +1095,7 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -1091,7 +1145,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="41" t="s">
         <v>66</v>
       </c>
       <c r="C4" s="5"/>
@@ -1101,7 +1155,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="41" t="s">
         <v>93</v>
       </c>
       <c r="C5" s="5"/>
@@ -1111,7 +1165,7 @@
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>92</v>
       </c>
       <c r="C6" s="5"/>
@@ -1128,8 +1182,12 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
@@ -7094,8 +7152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34:I40"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I44" sqref="I43:I44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -7205,10 +7263,10 @@
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="40">
+      <c r="I3" s="39">
         <v>42376</v>
       </c>
       <c r="J3" s="13"/>
@@ -7243,10 +7301,10 @@
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
-      <c r="H4" s="50" t="s">
+      <c r="H4" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="39">
         <v>42376</v>
       </c>
       <c r="J4" s="13"/>
@@ -7281,10 +7339,10 @@
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="40">
+      <c r="I5" s="39">
         <v>42376</v>
       </c>
       <c r="J5" s="13"/>
@@ -7319,10 +7377,10 @@
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
-      <c r="H6" s="50" t="s">
+      <c r="H6" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="39">
         <v>42376</v>
       </c>
       <c r="J6" s="13"/>
@@ -7357,10 +7415,10 @@
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="50" t="s">
+      <c r="H7" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="39">
         <v>42376</v>
       </c>
       <c r="J7" s="13"/>
@@ -7395,10 +7453,10 @@
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="12"/>
-      <c r="H8" s="50" t="s">
+      <c r="H8" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="39">
         <v>42376</v>
       </c>
       <c r="J8" s="13"/>
@@ -7465,10 +7523,10 @@
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="39">
         <v>42376</v>
       </c>
       <c r="J10" s="13"/>
@@ -7503,10 +7561,10 @@
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="50" t="s">
+      <c r="H11" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="39">
         <v>42376</v>
       </c>
       <c r="J11" s="13"/>
@@ -7541,10 +7599,10 @@
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
-      <c r="H12" s="50" t="s">
+      <c r="H12" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I12" s="40">
+      <c r="I12" s="39">
         <v>42376</v>
       </c>
       <c r="J12" s="13"/>
@@ -7579,10 +7637,10 @@
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="50" t="s">
+      <c r="H13" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I13" s="39">
         <v>42376</v>
       </c>
       <c r="J13" s="11"/>
@@ -7617,10 +7675,10 @@
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="50" t="s">
+      <c r="H14" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="40">
+      <c r="I14" s="39">
         <v>42376</v>
       </c>
       <c r="J14" s="11"/>
@@ -7655,10 +7713,10 @@
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
-      <c r="H15" s="50" t="s">
+      <c r="H15" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="40">
+      <c r="I15" s="39">
         <v>42376</v>
       </c>
       <c r="J15" s="11"/>
@@ -7693,10 +7751,10 @@
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="40">
+      <c r="I16" s="39">
         <v>42376</v>
       </c>
       <c r="J16" s="11"/>
@@ -7718,26 +7776,26 @@
       <c r="Z16" s="8"/>
     </row>
     <row r="17" spans="1:26" ht="81.75" customHeight="1">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="50" t="s">
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I17" s="39">
         <v>42376</v>
       </c>
-      <c r="J17" s="36"/>
+      <c r="J17" s="35"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
@@ -7788,32 +7846,32 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" spans="1:26" ht="34.5" customHeight="1">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="41" t="s">
+      <c r="C19" s="37"/>
+      <c r="D19" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="41" t="s">
+      <c r="F19" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="39" t="s">
+      <c r="H19" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="I19" s="44">
+      <c r="I19" s="43">
         <v>42376</v>
       </c>
-      <c r="J19" s="38"/>
+      <c r="J19" s="37"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
@@ -7864,32 +7922,32 @@
       <c r="Z20" s="8"/>
     </row>
     <row r="21" spans="1:26" ht="60" customHeight="1">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="39" t="s">
+      <c r="C21" s="37"/>
+      <c r="D21" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="39" t="s">
+      <c r="F21" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H21" s="41" t="s">
+      <c r="H21" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I21" s="39">
         <v>42497</v>
       </c>
-      <c r="J21" s="38"/>
+      <c r="J21" s="37"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
       <c r="M21" s="8"/>
@@ -7908,32 +7966,32 @@
       <c r="Z21" s="8"/>
     </row>
     <row r="22" spans="1:26" ht="60" customHeight="1">
-      <c r="A22" s="43" t="s">
+      <c r="A22" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="39" t="s">
+      <c r="C22" s="37"/>
+      <c r="D22" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="39" t="s">
+      <c r="F22" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G22" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I22" s="40">
+      <c r="I22" s="39">
         <v>42497</v>
       </c>
-      <c r="J22" s="38"/>
+      <c r="J22" s="37"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
@@ -7952,32 +8010,32 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" spans="1:26" ht="60" customHeight="1">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="39" t="s">
+      <c r="C23" s="37"/>
+      <c r="D23" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="39" t="s">
+      <c r="G23" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="41" t="s">
+      <c r="H23" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I23" s="39">
         <v>42497</v>
       </c>
-      <c r="J23" s="38"/>
+      <c r="J23" s="37"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
@@ -7996,32 +8054,32 @@
       <c r="Z23" s="8"/>
     </row>
     <row r="24" spans="1:26" ht="60" customHeight="1">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="39" t="s">
+      <c r="C24" s="37"/>
+      <c r="D24" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="39" t="s">
+      <c r="F24" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="39">
         <v>42497</v>
       </c>
-      <c r="J24" s="38"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
@@ -8040,32 +8098,32 @@
       <c r="Z24" s="8"/>
     </row>
     <row r="25" spans="1:26" ht="75">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B25" s="38" t="s">
+      <c r="B25" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="39" t="s">
+      <c r="C25" s="37"/>
+      <c r="D25" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="39" t="s">
+      <c r="F25" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="39" t="s">
+      <c r="G25" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="41" t="s">
+      <c r="H25" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="39">
         <v>42497</v>
       </c>
-      <c r="J25" s="38"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
@@ -8084,7 +8142,7 @@
       <c r="Z25" s="8"/>
     </row>
     <row r="26" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A26" s="45" t="s">
+      <c r="A26" s="44" t="s">
         <v>72</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -8096,7 +8154,7 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="46"/>
+      <c r="I26" s="45"/>
       <c r="J26" s="10"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
@@ -8116,32 +8174,32 @@
       <c r="Z26" s="8"/>
     </row>
     <row r="27" spans="1:26" ht="120" customHeight="1">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="39" t="s">
+      <c r="C27" s="37"/>
+      <c r="D27" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="F27" s="39" t="s">
+      <c r="F27" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="39" t="s">
+      <c r="G27" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H27" s="41" t="s">
+      <c r="H27" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="39">
         <v>42467</v>
       </c>
-      <c r="J27" s="38"/>
+      <c r="J27" s="37"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -8160,32 +8218,32 @@
       <c r="Z27" s="8"/>
     </row>
     <row r="28" spans="1:26" ht="124.5" customHeight="1">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="39" t="s">
+      <c r="C28" s="37"/>
+      <c r="D28" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="F28" s="39" t="s">
+      <c r="F28" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="39" t="s">
+      <c r="G28" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="41" t="s">
+      <c r="H28" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I28" s="40">
+      <c r="I28" s="39">
         <v>42467</v>
       </c>
-      <c r="J28" s="38"/>
+      <c r="J28" s="37"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8"/>
@@ -8204,32 +8262,32 @@
       <c r="Z28" s="8"/>
     </row>
     <row r="29" spans="1:26" ht="118.5" customHeight="1">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="39" t="s">
+      <c r="C29" s="37"/>
+      <c r="D29" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H29" s="41" t="s">
+      <c r="H29" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I29" s="40">
+      <c r="I29" s="39">
         <v>42467</v>
       </c>
-      <c r="J29" s="38"/>
+      <c r="J29" s="37"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8"/>
@@ -8248,32 +8306,32 @@
       <c r="Z29" s="8"/>
     </row>
     <row r="30" spans="1:26" ht="117.75" customHeight="1">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39" t="s">
+      <c r="C30" s="37"/>
+      <c r="D30" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="39" t="s">
+      <c r="E30" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="39" t="s">
+      <c r="F30" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H30" s="41" t="s">
+      <c r="H30" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="39">
         <v>42467</v>
       </c>
-      <c r="J30" s="38"/>
+      <c r="J30" s="37"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8"/>
@@ -8292,32 +8350,32 @@
       <c r="Z30" s="8"/>
     </row>
     <row r="31" spans="1:26" ht="120">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="39" t="s">
+      <c r="C31" s="37"/>
+      <c r="D31" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F31" s="39" t="s">
+      <c r="F31" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H31" s="41" t="s">
+      <c r="H31" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I31" s="40">
+      <c r="I31" s="39">
         <v>42467</v>
       </c>
-      <c r="J31" s="38"/>
+      <c r="J31" s="37"/>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8"/>
@@ -8336,32 +8394,32 @@
       <c r="Z31" s="8"/>
     </row>
     <row r="32" spans="1:26" ht="93.75" customHeight="1">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="C32" s="38"/>
-      <c r="D32" s="39" t="s">
+      <c r="C32" s="37"/>
+      <c r="D32" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="39" t="s">
+      <c r="E32" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="G32" s="39" t="s">
+      <c r="G32" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H32" s="41" t="s">
+      <c r="H32" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="I32" s="40">
+      <c r="I32" s="39">
         <v>42467</v>
       </c>
-      <c r="J32" s="38"/>
+      <c r="J32" s="37"/>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
@@ -8380,20 +8438,20 @@
       <c r="Z32" s="8"/>
     </row>
     <row r="33" spans="1:26" ht="24" customHeight="1">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="B33" s="51" t="s">
+      <c r="B33" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50"/>
+      <c r="H33" s="50"/>
+      <c r="I33" s="50"/>
+      <c r="J33" s="50"/>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
@@ -8412,32 +8470,32 @@
       <c r="Z33" s="8"/>
     </row>
     <row r="34" spans="1:26" ht="81" customHeight="1">
-      <c r="A34" s="52" t="s">
+      <c r="A34" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="B34" s="52" t="s">
+      <c r="B34" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="53" t="s">
+      <c r="C34" s="51"/>
+      <c r="D34" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="53" t="s">
+      <c r="E34" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="53" t="s">
+      <c r="F34" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G34" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="53" t="s">
+      <c r="H34" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I34" s="40">
+      <c r="I34" s="39">
         <v>42467</v>
       </c>
-      <c r="J34" s="53"/>
+      <c r="J34" s="52"/>
       <c r="K34" s="8"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
@@ -8456,32 +8514,32 @@
       <c r="Z34" s="8"/>
     </row>
     <row r="35" spans="1:26" ht="80.25" customHeight="1">
-      <c r="A35" s="52" t="s">
+      <c r="A35" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="C35" s="52"/>
-      <c r="D35" s="53" t="s">
+      <c r="C35" s="51"/>
+      <c r="D35" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="53" t="s">
+      <c r="E35" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F35" s="53" t="s">
+      <c r="F35" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="39" t="s">
+      <c r="G35" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H35" s="53" t="s">
+      <c r="H35" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I35" s="40">
+      <c r="I35" s="39">
         <v>42467</v>
       </c>
-      <c r="J35" s="53"/>
+      <c r="J35" s="52"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
@@ -8500,32 +8558,32 @@
       <c r="Z35" s="8"/>
     </row>
     <row r="36" spans="1:26" ht="57" customHeight="1">
-      <c r="A36" s="52" t="s">
+      <c r="A36" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="53" t="s">
+      <c r="C36" s="51"/>
+      <c r="D36" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="53" t="s">
+      <c r="E36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F36" s="53" t="s">
+      <c r="F36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="39" t="s">
+      <c r="G36" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H36" s="53" t="s">
+      <c r="H36" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I36" s="40">
+      <c r="I36" s="39">
         <v>42467</v>
       </c>
-      <c r="J36" s="53"/>
+      <c r="J36" s="52"/>
       <c r="K36" s="8"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
@@ -8544,32 +8602,32 @@
       <c r="Z36" s="8"/>
     </row>
     <row r="37" spans="1:26" ht="86.25" customHeight="1">
-      <c r="A37" s="52" t="s">
+      <c r="A37" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="51" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53" t="s">
+      <c r="C37" s="51"/>
+      <c r="D37" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="53" t="s">
+      <c r="E37" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="53" t="s">
+      <c r="F37" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="39" t="s">
+      <c r="G37" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H37" s="53" t="s">
+      <c r="H37" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I37" s="40">
+      <c r="I37" s="39">
         <v>42467</v>
       </c>
-      <c r="J37" s="53"/>
+      <c r="J37" s="52"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
@@ -8588,32 +8646,32 @@
       <c r="Z37" s="8"/>
     </row>
     <row r="38" spans="1:26" ht="79.5" customHeight="1">
-      <c r="A38" s="52" t="s">
+      <c r="A38" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="51" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="52"/>
-      <c r="D38" s="53" t="s">
+      <c r="C38" s="51"/>
+      <c r="D38" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="53" t="s">
+      <c r="E38" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F38" s="53" t="s">
+      <c r="F38" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G38" s="39" t="s">
+      <c r="G38" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H38" s="53" t="s">
+      <c r="H38" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I38" s="40">
+      <c r="I38" s="39">
         <v>42467</v>
       </c>
-      <c r="J38" s="53"/>
+      <c r="J38" s="52"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
@@ -8632,32 +8690,32 @@
       <c r="Z38" s="8"/>
     </row>
     <row r="39" spans="1:26" ht="90">
-      <c r="A39" s="52" t="s">
+      <c r="A39" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="B39" s="52" t="s">
+      <c r="B39" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="53" t="s">
+      <c r="C39" s="51"/>
+      <c r="D39" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="E39" s="53" t="s">
+      <c r="E39" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F39" s="53" t="s">
+      <c r="F39" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G39" s="39" t="s">
+      <c r="G39" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="53" t="s">
+      <c r="H39" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I39" s="40">
+      <c r="I39" s="39">
         <v>42467</v>
       </c>
-      <c r="J39" s="53"/>
+      <c r="J39" s="52"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
@@ -8676,32 +8734,32 @@
       <c r="Z39" s="8"/>
     </row>
     <row r="40" spans="1:26" ht="113.25" customHeight="1">
-      <c r="A40" s="52" t="s">
+      <c r="A40" s="51" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="51" t="s">
         <v>109</v>
       </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53" t="s">
+      <c r="C40" s="51"/>
+      <c r="D40" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E40" s="53" t="s">
+      <c r="E40" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="F40" s="53" t="s">
+      <c r="F40" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="G40" s="39" t="s">
+      <c r="G40" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="H40" s="53" t="s">
+      <c r="H40" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="I40" s="40">
+      <c r="I40" s="39">
         <v>42467</v>
       </c>
-      <c r="J40" s="53"/>
+      <c r="J40" s="52"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
@@ -8719,17 +8777,21 @@
       <c r="Y40" s="8"/>
       <c r="Z40" s="8"/>
     </row>
-    <row r="41" spans="1:26" ht="81.75" customHeight="1">
-      <c r="A41" s="30"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="25"/>
+    <row r="41" spans="1:26" ht="25.5" customHeight="1">
+      <c r="A41" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="10"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
@@ -8747,17 +8809,33 @@
       <c r="Y41" s="8"/>
       <c r="Z41" s="8"/>
     </row>
-    <row r="42" spans="1:26" ht="93.75" customHeight="1">
-      <c r="A42" s="30"/>
-      <c r="B42" s="26"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="25"/>
+    <row r="42" spans="1:26" ht="123" customHeight="1">
+      <c r="A42" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="37"/>
+      <c r="D42" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="F42" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="G42" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I42" s="39">
+        <v>42558</v>
+      </c>
+      <c r="J42" s="37"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
@@ -8776,16 +8854,32 @@
       <c r="Z42" s="8"/>
     </row>
     <row r="43" spans="1:26" ht="93.75" customHeight="1">
-      <c r="A43" s="30"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="25"/>
+      <c r="A43" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C43" s="37"/>
+      <c r="D43" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="E43" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H43" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I43" s="39">
+        <v>42558</v>
+      </c>
+      <c r="J43" s="37"/>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
@@ -8804,16 +8898,32 @@
       <c r="Z43" s="8"/>
     </row>
     <row r="44" spans="1:26" ht="94.5" customHeight="1">
-      <c r="A44" s="30"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="25"/>
+      <c r="A44" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="37"/>
+      <c r="D44" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="F44" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="G44" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H44" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="I44" s="39">
+        <v>42558</v>
+      </c>
+      <c r="J44" s="37"/>
       <c r="K44" s="8"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
@@ -8832,16 +8942,16 @@
       <c r="Z44" s="8"/>
     </row>
     <row r="45" spans="1:26" ht="96" customHeight="1">
-      <c r="A45" s="30"/>
-      <c r="B45" s="26"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="25"/>
+      <c r="A45" s="46"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="37"/>
       <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
@@ -8860,16 +8970,16 @@
       <c r="Z45" s="8"/>
     </row>
     <row r="46" spans="1:26">
-      <c r="A46" s="28"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="24"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="38"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="38"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="37"/>
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
@@ -8888,16 +8998,16 @@
       <c r="Z46" s="8"/>
     </row>
     <row r="47" spans="1:26" ht="94.5" customHeight="1">
-      <c r="A47" s="30"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="25"/>
+      <c r="A47" s="46"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="37"/>
       <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
@@ -8916,16 +9026,16 @@
       <c r="Z47" s="8"/>
     </row>
     <row r="48" spans="1:26" ht="93" customHeight="1">
-      <c r="A48" s="30"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="25"/>
+      <c r="A48" s="46"/>
+      <c r="B48" s="38"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="38"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="37"/>
       <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
@@ -9003,10 +9113,10 @@
       <c r="A51" s="30"/>
       <c r="B51" s="26"/>
       <c r="C51" s="25"/>
-      <c r="D51" s="34"/>
+      <c r="D51" s="33"/>
       <c r="E51" s="26"/>
       <c r="F51" s="26"/>
-      <c r="G51" s="35"/>
+      <c r="G51" s="34"/>
       <c r="H51" s="25"/>
       <c r="I51" s="27"/>
       <c r="J51" s="25"/>

</xml_diff>